<commit_message>
Ran new weighting options and renamed files.
</commit_message>
<xml_diff>
--- a/data/needle_3CH_3AA/02-22-2021_Test-Image-Subtraction/measured-arclength_fbg-camera.xlsx
+++ b/data/needle_3CH_3AA/02-22-2021_Test-Image-Subtraction/measured-arclength_fbg-camera.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="39">
   <si>
     <t>hole_num</t>
   </si>
@@ -152,7 +152,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -166,11 +166,29 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -178,6 +196,24 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -199,22 +235,22 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="19" t="s">
         <v>5</v>
       </c>
     </row>
@@ -226,7 +262,7 @@
         <v>75</v>
       </c>
       <c r="C2">
-        <v>74.999992494529408</v>
+        <v>74.99999129308685</v>
       </c>
       <c r="D2">
         <v>67.955426156112807</v>
@@ -246,7 +282,7 @@
         <v>80</v>
       </c>
       <c r="C3">
-        <v>79.999990931006138</v>
+        <v>79.999990191024295</v>
       </c>
       <c r="D3">
         <v>72.873138026097223</v>
@@ -266,7 +302,7 @@
         <v>85</v>
       </c>
       <c r="C4">
-        <v>84.999989914784919</v>
+        <v>84.999989148390796</v>
       </c>
       <c r="D4">
         <v>77.181105346631966</v>
@@ -286,7 +322,7 @@
         <v>90</v>
       </c>
       <c r="C5">
-        <v>89.99998704525035</v>
+        <v>89.999984966597395</v>
       </c>
       <c r="D5">
         <v>82.346955381237379</v>
@@ -306,7 +342,7 @@
         <v>75</v>
       </c>
       <c r="C6">
-        <v>74.999992665139331</v>
+        <v>74.999990816276494</v>
       </c>
       <c r="D6">
         <v>67.350467973433581</v>
@@ -326,7 +362,7 @@
         <v>80</v>
       </c>
       <c r="C7">
-        <v>79.999988675038466</v>
+        <v>79.999985039302942</v>
       </c>
       <c r="D7">
         <v>72.049255486370129</v>
@@ -346,7 +382,7 @@
         <v>85</v>
       </c>
       <c r="C8">
-        <v>84.999985037483825</v>
+        <v>84.999981287660205</v>
       </c>
       <c r="D8">
         <v>76.948909577356005</v>
@@ -366,7 +402,7 @@
         <v>90</v>
       </c>
       <c r="C9">
-        <v>89.999980070312063</v>
+        <v>89.999972202755757</v>
       </c>
       <c r="D9">
         <v>81.672841265763438</v>
@@ -386,7 +422,7 @@
         <v>75</v>
       </c>
       <c r="C10">
-        <v>74.999994802770146</v>
+        <v>74.999999693041332</v>
       </c>
       <c r="D10">
         <v>67.307305608845951</v>
@@ -406,7 +442,7 @@
         <v>80</v>
       </c>
       <c r="C11">
-        <v>79.999990815892673</v>
+        <v>79.999987392206549</v>
       </c>
       <c r="D11">
         <v>71.77928381411526</v>
@@ -426,7 +462,7 @@
         <v>85</v>
       </c>
       <c r="C12">
-        <v>84.999987420681677</v>
+        <v>84.999984033699235</v>
       </c>
       <c r="D12">
         <v>76.50126491227924</v>
@@ -446,7 +482,7 @@
         <v>90</v>
       </c>
       <c r="C13">
-        <v>89.999984781300398</v>
+        <v>89.999981396504253</v>
       </c>
       <c r="D13">
         <v>81.418484484796295</v>
@@ -493,78 +529,78 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="21" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="21" t="s">
         <v>7</v>
       </c>
       <c r="B2">
@@ -586,16 +622,16 @@
         <v>6</v>
       </c>
       <c r="H2">
-        <v>74.999992494529408</v>
+        <v>74.999990816276494</v>
       </c>
       <c r="I2">
-        <v>74.999993320812962</v>
+        <v>74.999993934134892</v>
       </c>
       <c r="J2">
-        <v>1.2862444398310795e-06</v>
+        <v>4.9930541320057655e-06</v>
       </c>
       <c r="K2">
-        <v>74.999994802770146</v>
+        <v>74.999999693041332</v>
       </c>
       <c r="L2">
         <v>67.307305608845951</v>
@@ -635,7 +671,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B3">
@@ -657,16 +693,16 @@
         <v>6</v>
       </c>
       <c r="H3">
-        <v>79.999988675038466</v>
+        <v>79.999985039302942</v>
       </c>
       <c r="I3">
-        <v>79.999990140645764</v>
+        <v>79.9999875408446</v>
       </c>
       <c r="J3">
-        <v>1.2705574880623968e-06</v>
+        <v>2.5790750624408201e-06</v>
       </c>
       <c r="K3">
-        <v>79.999990931006138</v>
+        <v>79.999990191024295</v>
       </c>
       <c r="L3">
         <v>71.77928381411526</v>
@@ -706,7 +742,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="21" t="s">
         <v>9</v>
       </c>
       <c r="B4">
@@ -728,16 +764,16 @@
         <v>6</v>
       </c>
       <c r="H4">
-        <v>84.999985037483825</v>
+        <v>84.999981287660205</v>
       </c>
       <c r="I4">
-        <v>84.99998745765015</v>
+        <v>84.999984823250074</v>
       </c>
       <c r="J4">
-        <v>2.4388606955271271e-06</v>
+        <v>3.9894002377171991e-06</v>
       </c>
       <c r="K4">
-        <v>84.999989914784919</v>
+        <v>84.999989148390796</v>
       </c>
       <c r="L4">
         <v>76.50126491227924</v>
@@ -777,7 +813,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="21" t="s">
         <v>10</v>
       </c>
       <c r="B5">
@@ -799,16 +835,16 @@
         <v>6</v>
       </c>
       <c r="H5">
-        <v>89.999980070312063</v>
+        <v>89.999972202755757</v>
       </c>
       <c r="I5">
-        <v>89.999983965620928</v>
+        <v>89.999979521952469</v>
       </c>
       <c r="J5">
-        <v>3.5582918325688778e-06</v>
+        <v>6.5851629926958643e-06</v>
       </c>
       <c r="K5">
-        <v>89.99998704525035</v>
+        <v>89.999984966597395</v>
       </c>
       <c r="L5">
         <v>81.418484484796295</v>
@@ -882,78 +918,78 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="23" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="23" t="s">
         <v>32</v>
       </c>
       <c r="B2">
@@ -975,16 +1011,16 @@
         <v>90</v>
       </c>
       <c r="H2">
-        <v>74.999992494529408</v>
+        <v>74.99999129308685</v>
       </c>
       <c r="I2">
-        <v>82.499990096392708</v>
+        <v>82.499988899774834</v>
       </c>
       <c r="J2">
-        <v>6.4549700019887473</v>
+        <v>6.454969658836867</v>
       </c>
       <c r="K2">
-        <v>89.99998704525035</v>
+        <v>89.999984966597395</v>
       </c>
       <c r="L2">
         <v>67.955426156112807</v>
@@ -1024,7 +1060,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="23" t="s">
         <v>33</v>
       </c>
       <c r="B3">
@@ -1046,16 +1082,16 @@
         <v>90</v>
       </c>
       <c r="H3">
-        <v>74.999992665139331</v>
+        <v>74.999990816276494</v>
       </c>
       <c r="I3">
-        <v>82.499986611993421</v>
+        <v>82.499982336498846</v>
       </c>
       <c r="J3">
-        <v>6.4549668961171269</v>
+        <v>6.4549645503585902</v>
       </c>
       <c r="K3">
-        <v>89.999980070312063</v>
+        <v>89.999972202755757</v>
       </c>
       <c r="L3">
         <v>67.350467973433581</v>
@@ -1095,7 +1131,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="23" t="s">
         <v>34</v>
       </c>
       <c r="B4">
@@ -1117,16 +1153,16 @@
         <v>90</v>
       </c>
       <c r="H4">
-        <v>74.999994802770146</v>
+        <v>74.999999693041332</v>
       </c>
       <c r="I4">
-        <v>82.499989455161227</v>
+        <v>82.499988128862839</v>
       </c>
       <c r="J4">
-        <v>6.4549679240606412</v>
+        <v>6.4549647238799484</v>
       </c>
       <c r="K4">
-        <v>89.999984781300398</v>
+        <v>89.999981396504253</v>
       </c>
       <c r="L4">
         <v>67.307305608845951</v>

</xml_diff>

<commit_message>
Updated needle insertion results using reliability weights
</commit_message>
<xml_diff>
--- a/data/needle_3CH_3AA/02-22-2021_Test-Image-Subtraction/measured-arclength_fbg-camera.xlsx
+++ b/data/needle_3CH_3AA/02-22-2021_Test-Image-Subtraction/measured-arclength_fbg-camera.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="39">
   <si>
     <t>hole_num</t>
   </si>
@@ -152,7 +152,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -184,11 +184,29 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -214,6 +232,24 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -235,22 +271,22 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="37" t="s">
         <v>5</v>
       </c>
     </row>
@@ -529,78 +565,78 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="Q1" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="R1" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="S1" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="T1" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="U1" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="V1" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="21" t="s">
+      <c r="W1" s="39" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="39" t="s">
         <v>7</v>
       </c>
       <c r="B2">
@@ -671,7 +707,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B3">
@@ -742,7 +778,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B4">
@@ -813,7 +849,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="39" t="s">
         <v>10</v>
       </c>
       <c r="B5">
@@ -918,78 +954,78 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="23" t="s">
+      <c r="P1" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="Q1" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="R1" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="23" t="s">
+      <c r="S1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="23" t="s">
+      <c r="T1" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="23" t="s">
+      <c r="U1" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="23" t="s">
+      <c r="V1" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="23" t="s">
+      <c r="W1" s="41" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="41" t="s">
         <v>32</v>
       </c>
       <c r="B2">
@@ -1060,7 +1096,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="41" t="s">
         <v>33</v>
       </c>
       <c r="B3">
@@ -1131,7 +1167,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="41" t="s">
         <v>34</v>
       </c>
       <c r="B4">

</xml_diff>

<commit_message>
Added needle shape image reprojections
</commit_message>
<xml_diff>
--- a/data/needle_3CH_3AA/02-22-2021_Test-Image-Subtraction/measured-arclength_fbg-camera.xlsx
+++ b/data/needle_3CH_3AA/02-22-2021_Test-Image-Subtraction/measured-arclength_fbg-camera.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="39">
   <si>
     <t>hole_num</t>
   </si>
@@ -152,7 +152,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="67">
     <border>
       <left/>
       <right/>
@@ -202,11 +202,35 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -250,6 +274,30 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="64" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="66" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -271,22 +319,22 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="61" t="s">
         <v>5</v>
       </c>
     </row>
@@ -565,78 +613,78 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="J1" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="L1" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="Q1" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="39" t="s">
+      <c r="S1" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="39" t="s">
+      <c r="T1" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="39" t="s">
+      <c r="U1" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="39" t="s">
+      <c r="V1" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="39" t="s">
+      <c r="W1" s="63" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="63" t="s">
         <v>7</v>
       </c>
       <c r="B2">
@@ -707,7 +755,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="63" t="s">
         <v>8</v>
       </c>
       <c r="B3">
@@ -778,7 +826,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="63" t="s">
         <v>9</v>
       </c>
       <c r="B4">
@@ -849,7 +897,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="63" t="s">
         <v>10</v>
       </c>
       <c r="B5">
@@ -954,78 +1002,78 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="K1" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="L1" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="41" t="s">
+      <c r="N1" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="41" t="s">
+      <c r="O1" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="41" t="s">
+      <c r="P1" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="41" t="s">
+      <c r="Q1" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="41" t="s">
+      <c r="R1" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="41" t="s">
+      <c r="S1" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="41" t="s">
+      <c r="T1" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="41" t="s">
+      <c r="U1" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="41" t="s">
+      <c r="V1" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="41" t="s">
+      <c r="W1" s="65" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="65" t="s">
         <v>32</v>
       </c>
       <c r="B2">
@@ -1096,7 +1144,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="65" t="s">
         <v>33</v>
       </c>
       <c r="B3">
@@ -1167,7 +1215,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="65" t="s">
         <v>34</v>
       </c>
       <c r="B4">

</xml_diff>